<commit_message>
Translate + clean data
</commit_message>
<xml_diff>
--- a/data/raw/Forms-Results-Raw.xlsx
+++ b/data/raw/Forms-Results-Raw.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="157">
   <si>
     <t>ID</t>
   </si>
@@ -221,7 +221,7 @@
     <t>España</t>
   </si>
   <si>
-    <t>Studiar y aprender, Trabajo</t>
+    <t>Studying or learning, Work/professional tasks</t>
   </si>
   <si>
     <t>para las matematicas</t>
@@ -233,9 +233,6 @@
     <t>Andorra</t>
   </si>
   <si>
-    <t>Trabajo</t>
-  </si>
-  <si>
     <t>Si</t>
   </si>
   <si>
@@ -248,7 +245,7 @@
     <t>Jubilada</t>
   </si>
   <si>
-    <t>Entretenimiento</t>
+    <t>Entertainment</t>
   </si>
   <si>
     <t>35-44</t>
@@ -257,7 +254,7 @@
     <t>Autónoma, administrativa</t>
   </si>
   <si>
-    <t>Trabajo, Otros</t>
+    <t>Work/professional tasks, Others</t>
   </si>
   <si>
     <t>Organizar viajes</t>
@@ -266,7 +263,7 @@
     <t>Arquitecta</t>
   </si>
   <si>
-    <t>Trabajo, Creacion de contenido para redes sociales</t>
+    <t>Work/professional tasks, Social media content</t>
   </si>
   <si>
     <t>55-64</t>
@@ -287,7 +284,7 @@
     <t>Reino Unido</t>
   </si>
   <si>
-    <t>Studiar y aprender, Escribir o Arte</t>
+    <t>Studying or learning, Creative writing or art</t>
   </si>
   <si>
     <t>Médico</t>
@@ -299,13 +296,13 @@
     <t>Empresario</t>
   </si>
   <si>
-    <t>Studiar y aprender, Trabajo, Creacion de contenido para redes sociales</t>
+    <t>Studying or learning, Work/professional tasks, Social media content</t>
   </si>
   <si>
     <t>Maestra</t>
   </si>
   <si>
-    <t>Otros</t>
+    <t>Others</t>
   </si>
   <si>
     <t>RRHH</t>
@@ -320,9 +317,6 @@
     <t>Pensionista</t>
   </si>
   <si>
-    <t>No la uso</t>
-  </si>
-  <si>
     <t xml:space="preserve">Odontóloga </t>
   </si>
   <si>
@@ -356,13 +350,13 @@
     <t>Ama de casa</t>
   </si>
   <si>
-    <t>Studiar y aprender, Entretenimiento</t>
+    <t>Studying or learning, Entertainment</t>
   </si>
   <si>
     <t>Cualquiera que me ayude a resolver problemas matematicos de manera exacta</t>
   </si>
   <si>
-    <t>Studiar y aprender, Creacion de contenido para redes sociales, Entretenimiento</t>
+    <t>Studying or learning, Social media content, Entertainment</t>
   </si>
   <si>
     <t>Contador</t>
@@ -371,16 +365,13 @@
     <t xml:space="preserve">Argentina </t>
   </si>
   <si>
-    <t>Studiar y aprender</t>
-  </si>
-  <si>
     <t>Nada</t>
   </si>
   <si>
     <t>Empleada</t>
   </si>
   <si>
-    <t>Studiar y aprender, Trabajo, Entretenimiento</t>
+    <t>Studying or learning, Work/professional tasks, Entertainment</t>
   </si>
   <si>
     <t>Una app para crear películas 😎</t>
@@ -389,19 +380,19 @@
     <t xml:space="preserve">Mecanico </t>
   </si>
   <si>
-    <t>Studiar y aprender, Entretenimiento, Otros</t>
-  </si>
-  <si>
-    <t>Una IA que ayudara con los procesos de conección con la Ecu de un vehiculo ya que dependiendo por ej del escaner que se use para ver las fallas de un vehiculo puede o no obtener acceso a los datos del motor (Esto tambien varia dependiendo de que marca sea el vehiculo). Seria practico un escaner que posea una IA y que esta ayudara a realizar la coneccion entre otros procesos.</t>
+    <t>Studying or learning, Entertainment, Others</t>
+  </si>
+  <si>
+    <t>Una IA que ayudara con los procesos de conección con la Ecu de un vehiculo ya que dependiendo por ej del escaner que se use para ver las fallas de un vehiculo puede o no obtener acceso a los datos del motor (Esto tambien varia dependiendo de que marca sea el vehiculo). Seria practico un escaner que posea una IA y que esta ayudara a realizar la coneccion entre Others procesos.</t>
   </si>
   <si>
     <t>Jefe de soporte técnico</t>
   </si>
   <si>
-    <t>Studiar y aprender, Trabajo, Otros</t>
-  </si>
-  <si>
-    <t>Studiar y aprender, Trabajo, Escribir o Arte</t>
+    <t>Studying or learning, Work/professional tasks, Others</t>
+  </si>
+  <si>
+    <t>Studying or learning, Work/professional tasks, Creative writing or art</t>
   </si>
   <si>
     <t>Una aplicación para tomar decisiones políticas y o condenatorias, quizá haya menos corrupción y justicia, pero quien sabe.</t>
@@ -419,7 +410,7 @@
     <t xml:space="preserve">Una IA que recopile todos los estudios y avances médicos por más nuevos o viejos que sean y que los puede traducir a diversos idiomas </t>
   </si>
   <si>
-    <t>Studiar y aprender, Otros</t>
+    <t>Studying or learning, Others</t>
   </si>
   <si>
     <t>Soporte it</t>
@@ -461,7 +452,7 @@
     <t>Desarrollador de software</t>
   </si>
   <si>
-    <t>Studiar y aprender, Trabajo, Entretenimiento, Otros</t>
+    <t>Studying or learning, Work/professional tasks, Entertainment, Others</t>
   </si>
   <si>
     <t>Gestion</t>
@@ -497,7 +488,7 @@
     <t>Colombia</t>
   </si>
   <si>
-    <t>Studiar y aprender, Escribir o Arte, Entretenimiento</t>
+    <t>Studying or learning, Creative writing or art, Entertainment</t>
   </si>
   <si>
     <t>IA para monitoreo de salud, actividad física o alguna aplicación útil para el campo de la salud.</t>
@@ -509,13 +500,13 @@
     <t>Me gustaria una aplicación de organización de viajes según intereses y criterio del usuario</t>
   </si>
   <si>
-    <t>Trabajo, Entretenimiento</t>
+    <t>Work/professional tasks, Entertainment</t>
   </si>
   <si>
     <t>Por ahora no se me ocurre ninguna</t>
   </si>
   <si>
-    <t>Entretenimiento, Otros</t>
+    <t>Entertainment, Others</t>
   </si>
 </sst>
 </file>
@@ -659,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -705,6 +696,9 @@
       <alignment horizontal="right" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1548,7 +1542,7 @@
       <c r="G11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="16" t="s">
         <v>61</v>
       </c>
       <c r="I11" s="6" t="s">
@@ -1601,35 +1595,35 @@
       <c r="G12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>65</v>
+      <c r="H12" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="I12" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q12" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="P12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q12" s="10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="13">
@@ -1637,10 +1631,10 @@
         <v>11.0</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>19</v>
@@ -1654,17 +1648,17 @@
       <c r="G13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>70</v>
+      <c r="H13" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L13" s="16" t="s">
         <v>25</v>
@@ -1688,10 +1682,10 @@
         <v>12.0</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>19</v>
@@ -1705,17 +1699,17 @@
       <c r="G14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>73</v>
+      <c r="H14" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>27</v>
@@ -1733,7 +1727,7 @@
         <v>27</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15">
@@ -1744,7 +1738,7 @@
         <v>17</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>19</v>
@@ -1758,14 +1752,14 @@
       <c r="G15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>76</v>
+      <c r="H15" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>32</v>
@@ -1792,16 +1786,16 @@
         <v>14.0</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>60</v>
@@ -1809,11 +1803,11 @@
       <c r="G16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="9" t="s">
         <v>61</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>32</v>
@@ -1843,10 +1837,10 @@
         <v>15.0</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>29</v>
@@ -1860,11 +1854,11 @@
       <c r="G17" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>65</v>
+      <c r="H17" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>32</v>
@@ -1888,7 +1882,7 @@
         <v>33</v>
       </c>
       <c r="Q17" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
@@ -1908,19 +1902,19 @@
         <v>20</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>83</v>
+      <c r="H18" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>32</v>
@@ -1947,16 +1941,16 @@
         <v>17.0</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>60</v>
@@ -1964,14 +1958,14 @@
       <c r="G19" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>65</v>
+      <c r="H19" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="I19" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>32</v>
@@ -1992,7 +1986,7 @@
         <v>26</v>
       </c>
       <c r="Q19" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20">
@@ -2000,10 +1994,10 @@
         <v>18.0</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>29</v>
@@ -2017,17 +2011,17 @@
       <c r="G20" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>87</v>
+      <c r="H20" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>27</v>
@@ -2054,7 +2048,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>19</v>
@@ -2068,14 +2062,14 @@
       <c r="G21" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>89</v>
+      <c r="H21" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>32</v>
@@ -2105,7 +2099,7 @@
         <v>39</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>19</v>
@@ -2114,19 +2108,19 @@
         <v>36</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="8" t="s">
-        <v>65</v>
+      <c r="H22" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>32</v>
@@ -2147,7 +2141,7 @@
         <v>27</v>
       </c>
       <c r="Q22" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23">
@@ -2155,10 +2149,10 @@
         <v>21.0</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>29</v>
@@ -2172,14 +2166,14 @@
       <c r="G23" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>94</v>
+      <c r="H23" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>32</v>
@@ -2209,7 +2203,7 @@
         <v>17</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>19</v>
@@ -2223,14 +2217,14 @@
       <c r="G24" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H24" s="8" t="s">
-        <v>70</v>
+      <c r="H24" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K24" s="8" t="s">
         <v>32</v>
@@ -2251,7 +2245,7 @@
         <v>33</v>
       </c>
       <c r="Q24" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25">
@@ -2259,16 +2253,16 @@
         <v>23.0</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>60</v>
@@ -2276,11 +2270,11 @@
       <c r="G25" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>89</v>
+      <c r="H25" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>32</v>
@@ -2304,7 +2298,7 @@
         <v>27</v>
       </c>
       <c r="Q25" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26">
@@ -2315,7 +2309,7 @@
         <v>39</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>19</v>
@@ -2324,22 +2318,22 @@
         <v>36</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="8" t="s">
-        <v>65</v>
+      <c r="H26" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L26" s="9" t="s">
         <v>38</v>
@@ -2357,7 +2351,7 @@
         <v>33</v>
       </c>
       <c r="Q26" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27">
@@ -2368,7 +2362,7 @@
         <v>39</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>19</v>
@@ -2377,19 +2371,19 @@
         <v>36</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G27" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>65</v>
+      <c r="H27" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>32</v>
@@ -2416,34 +2410,34 @@
         <v>26.0</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="8" t="s">
-        <v>89</v>
+      <c r="H28" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L28" s="9" t="s">
         <v>25</v>
@@ -2479,22 +2473,22 @@
         <v>36</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>106</v>
+      <c r="H29" s="16" t="s">
+        <v>104</v>
       </c>
       <c r="I29" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L29" s="6" t="s">
         <v>27</v>
@@ -2512,7 +2506,7 @@
         <v>27</v>
       </c>
       <c r="Q29" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30">
@@ -2532,22 +2526,22 @@
         <v>36</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="8" t="s">
-        <v>108</v>
+      <c r="H30" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>27</v>
@@ -2574,7 +2568,7 @@
         <v>17</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>29</v>
@@ -2583,22 +2577,22 @@
         <v>36</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G31" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>111</v>
+      <c r="H31" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L31" s="16" t="s">
         <v>26</v>
@@ -2616,7 +2610,7 @@
         <v>33</v>
       </c>
       <c r="Q31" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32">
@@ -2627,7 +2621,7 @@
         <v>39</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>19</v>
@@ -2636,22 +2630,22 @@
         <v>59</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="8" t="s">
-        <v>114</v>
+      <c r="H32" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>32</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>27</v>
@@ -2669,7 +2663,7 @@
         <v>25</v>
       </c>
       <c r="Q32" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33">
@@ -2689,16 +2683,16 @@
         <v>59</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G33" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H33" s="6" t="s">
-        <v>106</v>
+      <c r="H33" s="16" t="s">
+        <v>104</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>32</v>
@@ -2722,7 +2716,7 @@
         <v>25</v>
       </c>
       <c r="Q33" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34">
@@ -2733,7 +2727,7 @@
         <v>39</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>29</v>
@@ -2742,19 +2736,19 @@
         <v>36</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H34" s="8" t="s">
-        <v>117</v>
+      <c r="H34" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K34" s="8" t="s">
         <v>32</v>
@@ -2774,8 +2768,8 @@
       <c r="P34" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q34" s="10" t="s">
-        <v>118</v>
+      <c r="Q34" s="17" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="35">
@@ -2783,10 +2777,10 @@
         <v>33.0</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>29</v>
@@ -2795,16 +2789,16 @@
         <v>36</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>120</v>
+      <c r="H35" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>32</v>
@@ -2837,7 +2831,7 @@
         <v>17</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>29</v>
@@ -2846,19 +2840,19 @@
         <v>36</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H36" s="8" t="s">
-        <v>121</v>
+      <c r="H36" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K36" s="8" t="s">
         <v>32</v>
@@ -2879,7 +2873,7 @@
         <v>27</v>
       </c>
       <c r="Q36" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37">
@@ -2899,19 +2893,19 @@
         <v>36</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>87</v>
+      <c r="H37" s="16" t="s">
+        <v>86</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K37" s="6" t="s">
         <v>32</v>
@@ -2947,25 +2941,25 @@
         <v>19</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="8" t="s">
-        <v>111</v>
+      <c r="H38" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J38" s="8" t="s">
         <v>32</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L38" s="8" t="s">
         <v>27</v>
@@ -2989,10 +2983,10 @@
         <v>37.0</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>19</v>
@@ -3001,19 +2995,19 @@
         <v>36</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H39" s="6" t="s">
-        <v>65</v>
+      <c r="H39" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K39" s="6" t="s">
         <v>32</v>
@@ -3040,10 +3034,10 @@
         <v>38.0</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>19</v>
@@ -3052,22 +3046,22 @@
         <v>36</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H40" s="8" t="s">
-        <v>94</v>
+      <c r="H40" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L40" s="9" t="s">
         <v>38</v>
@@ -3085,7 +3079,7 @@
         <v>33</v>
       </c>
       <c r="Q40" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41">
@@ -3105,19 +3099,19 @@
         <v>59</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H41" s="6" t="s">
-        <v>106</v>
+      <c r="H41" s="16" t="s">
+        <v>104</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K41" s="6" t="s">
         <v>32</v>
@@ -3138,7 +3132,7 @@
         <v>27</v>
       </c>
       <c r="Q41" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42">
@@ -3158,22 +3152,22 @@
         <v>36</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H42" s="8" t="s">
-        <v>127</v>
+      <c r="H42" s="9" t="s">
+        <v>124</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J42" s="8" t="s">
         <v>32</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L42" s="8" t="s">
         <v>27</v>
@@ -3200,7 +3194,7 @@
         <v>17</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>19</v>
@@ -3209,19 +3203,19 @@
         <v>36</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G43" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="H43" s="16" t="s">
         <v>61</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K43" s="6" t="s">
         <v>32</v>
@@ -3242,7 +3236,7 @@
         <v>27</v>
       </c>
       <c r="Q43" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44">
@@ -3253,7 +3247,7 @@
         <v>17</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>19</v>
@@ -3267,17 +3261,17 @@
       <c r="G44" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H44" s="8" t="s">
-        <v>114</v>
+      <c r="H44" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J44" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L44" s="8" t="s">
         <v>27</v>
@@ -3295,7 +3289,7 @@
         <v>26</v>
       </c>
       <c r="Q44" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45">
@@ -3306,7 +3300,7 @@
         <v>17</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>29</v>
@@ -3320,14 +3314,14 @@
       <c r="G45" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H45" s="6" t="s">
-        <v>94</v>
+      <c r="H45" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K45" s="6" t="s">
         <v>32</v>
@@ -3357,7 +3351,7 @@
         <v>17</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>29</v>
@@ -3366,19 +3360,19 @@
         <v>36</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H46" s="8" t="s">
+      <c r="H46" s="9" t="s">
         <v>61</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J46" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K46" s="8" t="s">
         <v>32</v>
@@ -3408,7 +3402,7 @@
         <v>39</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>29</v>
@@ -3417,13 +3411,13 @@
         <v>36</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H47" s="6" t="s">
-        <v>83</v>
+      <c r="H47" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>32</v>
@@ -3450,7 +3444,7 @@
         <v>33</v>
       </c>
       <c r="Q47" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48">
@@ -3458,10 +3452,10 @@
         <v>46.0</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>29</v>
@@ -3470,19 +3464,19 @@
         <v>36</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H48" s="8" t="s">
-        <v>114</v>
+      <c r="H48" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K48" s="8" t="s">
         <v>32</v>
@@ -3503,7 +3497,7 @@
         <v>33</v>
       </c>
       <c r="Q48" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49">
@@ -3511,10 +3505,10 @@
         <v>47.0</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>19</v>
@@ -3523,13 +3517,13 @@
         <v>59</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H49" s="6" t="s">
-        <v>94</v>
+      <c r="H49" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>32</v>
@@ -3538,7 +3532,7 @@
         <v>32</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L49" s="6" t="s">
         <v>27</v>
@@ -3562,10 +3556,10 @@
         <v>48.0</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>19</v>
@@ -3574,16 +3568,16 @@
         <v>36</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H50" s="8" t="s">
-        <v>141</v>
+      <c r="H50" s="9" t="s">
+        <v>138</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J50" s="8" t="s">
         <v>32</v>
@@ -3613,7 +3607,7 @@
         <v>49.0</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>35</v>
@@ -3630,14 +3624,14 @@
       <c r="G51" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="H51" s="6" t="s">
-        <v>89</v>
+      <c r="H51" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K51" s="6" t="s">
         <v>32</v>
@@ -3664,10 +3658,10 @@
         <v>50.0</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>29</v>
@@ -3681,11 +3675,11 @@
       <c r="G52" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H52" s="8" t="s">
-        <v>73</v>
+      <c r="H52" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J52" s="8" t="s">
         <v>32</v>
@@ -3709,7 +3703,7 @@
         <v>26</v>
       </c>
       <c r="Q52" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53">
@@ -3717,10 +3711,10 @@
         <v>51.0</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>29</v>
@@ -3729,22 +3723,22 @@
         <v>36</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G53" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H53" s="6" t="s">
-        <v>114</v>
+      <c r="H53" s="16" t="s">
+        <v>111</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L53" s="16" t="s">
         <v>25</v>
@@ -3762,7 +3756,7 @@
         <v>26</v>
       </c>
       <c r="Q53" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54">
@@ -3770,10 +3764,10 @@
         <v>52.0</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>29</v>
@@ -3782,13 +3776,13 @@
         <v>59</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H54" s="8" t="s">
-        <v>70</v>
+      <c r="H54" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>32</v>
@@ -3824,13 +3818,13 @@
         <v>17</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>60</v>
@@ -3838,14 +3832,14 @@
       <c r="G55" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H55" s="6" t="s">
-        <v>94</v>
+      <c r="H55" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="I55" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>32</v>
@@ -3866,7 +3860,7 @@
         <v>26</v>
       </c>
       <c r="Q55" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56">
@@ -3877,13 +3871,13 @@
         <v>17</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>64</v>
@@ -3891,14 +3885,14 @@
       <c r="G56" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H56" s="8" t="s">
-        <v>73</v>
+      <c r="H56" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="I56" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J56" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K56" s="8" t="s">
         <v>32</v>
@@ -3919,7 +3913,7 @@
         <v>27</v>
       </c>
       <c r="Q56" s="10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57">
@@ -3939,19 +3933,19 @@
         <v>36</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G57" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="H57" s="6" t="s">
-        <v>94</v>
+      <c r="H57" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="I57" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K57" s="6" t="s">
         <v>32</v>
@@ -3990,22 +3984,22 @@
         <v>36</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G58" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H58" s="8" t="s">
-        <v>153</v>
+      <c r="H58" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="I58" s="8" t="s">
         <v>32</v>
       </c>
       <c r="J58" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L58" s="9" t="s">
         <v>25</v>
@@ -4023,7 +4017,7 @@
         <v>33</v>
       </c>
       <c r="Q58" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59">
@@ -4034,7 +4028,7 @@
         <v>17</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>19</v>
@@ -4048,17 +4042,17 @@
       <c r="G59" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H59" s="6" t="s">
-        <v>65</v>
+      <c r="H59" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="I59" s="6" t="s">
         <v>32</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L59" s="16" t="s">
         <v>38</v>
@@ -4076,7 +4070,7 @@
         <v>33</v>
       </c>
       <c r="Q59" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60">
@@ -4101,17 +4095,17 @@
       <c r="G60" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H60" s="8" t="s">
-        <v>157</v>
+      <c r="H60" s="9" t="s">
+        <v>154</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J60" s="8" t="s">
         <v>32</v>
       </c>
       <c r="K60" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L60" s="8" t="s">
         <v>27</v>
@@ -4129,7 +4123,7 @@
         <v>25</v>
       </c>
       <c r="Q60" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61">
@@ -4145,26 +4139,26 @@
       <c r="D61" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E61" s="17" t="s">
-        <v>99</v>
+      <c r="E61" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="F61" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G61" s="17" t="s">
+      <c r="G61" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H61" s="13" t="s">
-        <v>159</v>
+      <c r="H61" s="18" t="s">
+        <v>156</v>
       </c>
       <c r="I61" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J61" s="13" t="s">
         <v>32</v>
       </c>
       <c r="K61" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L61" s="13" t="s">
         <v>27</v>
@@ -4172,16 +4166,16 @@
       <c r="M61" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="N61" s="17" t="s">
+      <c r="N61" s="18" t="s">
         <v>25</v>
       </c>
       <c r="O61" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="P61" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q61" s="18"/>
+      <c r="P61" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q61" s="19"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>